<commit_message>
Finalized CAD and added Visualize
</commit_message>
<xml_diff>
--- a/Electrical/PCB_Project/Documents/Project Outputs for ROBOT_PCB_PROJECT/ROBOT_PCB_PROJECT.xlsx
+++ b/Electrical/PCB_Project/Documents/Project Outputs for ROBOT_PCB_PROJECT/ROBOT_PCB_PROJECT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan Heddle\OneDrive\Desktop\AI-Robot\PCB\PCB_Project\Project Outputs for AI_PCB_PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan Heddle\OneDrive\Desktop\Ergos-Dynamic-Humanoid-Platform\electrical\PCB_Project\Documents\Project Outputs for ROBOT_PCB_PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DDE6A4-B2C6-44C0-8153-606438C38B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ED6EE7-F7E6-46F3-BBFC-6700AE5E11B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{308192D4-E0FA-4898-8827-247AC0BD94FB}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="291">
   <si>
     <t>Line #</t>
   </si>
@@ -428,9 +428,6 @@
     <t>21</t>
   </si>
   <si>
-    <t>XAL6060-472MEB</t>
-  </si>
-  <si>
     <t>Power inductor, shielded, 20% tol, SMT, RoHS, halogen-f</t>
   </si>
   <si>
@@ -614,9 +611,6 @@
     <t>Vishay Dale</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
@@ -821,7 +815,103 @@
     <t>JLCPCB</t>
   </si>
   <si>
-    <t>C7421717</t>
+    <t>67-1356-2-ND</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>450-1650-ND</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>311-1140-2-ND</t>
+  </si>
+  <si>
+    <t>490-1427-2-ND</t>
+  </si>
+  <si>
+    <t>490-3261-2-ND</t>
+  </si>
+  <si>
+    <t>SMBJ13A-FDITR-ND</t>
+  </si>
+  <si>
+    <t>Torex</t>
+  </si>
+  <si>
+    <t>865-XBS053V15R-G</t>
+  </si>
+  <si>
+    <t>455-2248-ND</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>FIT0588</t>
+  </si>
+  <si>
+    <t>DFRobot</t>
+  </si>
+  <si>
+    <t>1738-1438-ND</t>
+  </si>
+  <si>
+    <t>Pheonix Contact</t>
+  </si>
+  <si>
+    <t>277-17516-ND</t>
+  </si>
+  <si>
+    <t>Harwin Inc.</t>
+  </si>
+  <si>
+    <t>952-2262-ND</t>
+  </si>
+  <si>
+    <t>XAL6060-472MEC</t>
+  </si>
+  <si>
+    <t>Coilcraft</t>
+  </si>
+  <si>
+    <t>994-XAL6060-472MEC</t>
+  </si>
+  <si>
+    <t>541-100KLTR-ND</t>
+  </si>
+  <si>
+    <t>311-105KMTR-ND</t>
+  </si>
+  <si>
+    <t>YAG2428TR-ND</t>
+  </si>
+  <si>
+    <t>YAG2524TR-ND</t>
+  </si>
+  <si>
+    <t>5407-ESP32-S3-WROOM-1-N4R2TR-ND</t>
+  </si>
+  <si>
+    <t>Espressif Systems</t>
+  </si>
+  <si>
+    <t>828-BMI323TR-ND</t>
+  </si>
+  <si>
+    <t>Bosch Sensortec</t>
+  </si>
+  <si>
+    <t>296-16845-2-ND</t>
+  </si>
+  <si>
+    <t>296-32243-2-ND</t>
+  </si>
+  <si>
+    <t>WM1399TR-ND</t>
   </si>
 </sst>
 </file>
@@ -878,12 +968,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1220,17 +1314,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03E2E66-A513-4405-B7A1-5B2288B349FD}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.42578125" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="2" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="27.42578125" customWidth="1"/>
@@ -1242,48 +1336,48 @@
     <col min="14" max="14" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>259</v>
+      <c r="N1" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1302,7 +1396,7 @@
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1314,10 +1408,18 @@
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="J2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.44</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1332,17 +1434,31 @@
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="G3" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1360,7 +1476,7 @@
       <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1372,10 +1488,18 @@
       <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="J4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.23</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1393,7 +1517,7 @@
       <c r="E5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1411,10 +1535,10 @@
       <c r="K5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="3">
         <v>0.82506999999999997</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="3">
         <v>1.65</v>
       </c>
     </row>
@@ -1434,7 +1558,7 @@
       <c r="E6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -1452,10 +1576,10 @@
       <c r="K6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="3">
         <v>1.538E-2</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="3">
         <v>1.538E-2</v>
       </c>
     </row>
@@ -1475,7 +1599,7 @@
       <c r="E7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1493,10 +1617,10 @@
       <c r="K7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="3">
         <v>0.13983999999999999</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="3">
         <v>0.13983999999999999</v>
       </c>
     </row>
@@ -1516,7 +1640,7 @@
       <c r="E8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1534,10 +1658,10 @@
       <c r="K8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="3">
         <v>0.72718000000000005</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="3">
         <v>1.45</v>
       </c>
     </row>
@@ -1557,7 +1681,7 @@
       <c r="E9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>3</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1575,10 +1699,10 @@
       <c r="K9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="3">
         <v>0.30764999999999998</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="3">
         <v>0.92296</v>
       </c>
     </row>
@@ -1598,16 +1722,30 @@
       <c r="E10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="G10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1625,7 +1763,7 @@
       <c r="E11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1643,10 +1781,10 @@
       <c r="K11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="3">
         <v>0.30764999999999998</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="3">
         <v>0.30764999999999998</v>
       </c>
     </row>
@@ -1666,7 +1804,7 @@
       <c r="E12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1684,10 +1822,10 @@
       <c r="K12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="3">
         <v>0.32163999999999998</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="3">
         <v>0.32163999999999998</v>
       </c>
     </row>
@@ -1707,16 +1845,30 @@
       <c r="E13" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="G13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1731,17 +1883,31 @@
       <c r="D14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
         <v>4</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+      <c r="G14" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1.1200000000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1759,16 +1925,30 @@
       <c r="E15" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="G15" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1.07</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1.07</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1786,7 +1966,7 @@
       <c r="E16" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <v>4</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1804,14 +1984,14 @@
       <c r="K16" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="3">
         <v>1.06</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="3">
         <v>4.22</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>105</v>
       </c>
@@ -1824,19 +2004,33 @@
       <c r="D17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
         <v>4</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G17" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>109</v>
       </c>
@@ -1849,19 +2043,33 @@
       <c r="D18" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G18" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="L18" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="M18" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -1874,19 +2082,33 @@
       <c r="D19" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3">
         <v>2</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G19" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1017505</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>116</v>
       </c>
@@ -1902,7 +2124,7 @@
       <c r="E20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="3">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -1920,14 +2142,14 @@
       <c r="K20" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20" s="3">
         <v>0.96492</v>
       </c>
-      <c r="M20" s="1">
+      <c r="M20" s="3">
         <v>0.96492</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>123</v>
       </c>
@@ -1943,71 +2165,96 @@
       <c r="E21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="3">
         <v>2</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G21" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="L22" s="3">
+        <v>6.82</v>
+      </c>
+      <c r="M22" s="3">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="3">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="H23" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>19</v>
@@ -2016,121 +2263,121 @@
         <v>36</v>
       </c>
       <c r="K23" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.93694999999999995</v>
+      </c>
+      <c r="M23" s="3">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="L23" s="1">
-        <v>0.93694999999999995</v>
-      </c>
-      <c r="M23" s="1">
-        <v>1.87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="3">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F24" s="1">
-        <v>5</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="L24" s="3">
+        <v>8.3899999999999999E-3</v>
+      </c>
+      <c r="M24" s="3">
+        <v>4.1950000000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="L24" s="1">
-        <v>8.3899999999999999E-3</v>
-      </c>
-      <c r="M24" s="1">
-        <v>4.1950000000000001E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="3">
+        <v>4</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F25" s="1">
-        <v>4</v>
-      </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="2" t="s">
+      <c r="K25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L25" s="3">
+        <v>2.66E-3</v>
+      </c>
+      <c r="M25" s="3">
+        <v>26.57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="K25" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="L25" s="1">
-        <v>2.66E-3</v>
-      </c>
-      <c r="M25" s="1">
-        <v>26.57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="F26" s="3">
         <v>6</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>19</v>
@@ -2139,39 +2386,39 @@
         <v>58</v>
       </c>
       <c r="K26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L26" s="3">
+        <v>4.0550000000000003E-2</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0.40554000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="L26" s="1">
-        <v>4.0550000000000003E-2</v>
-      </c>
-      <c r="M26" s="1">
-        <v>0.40554000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>19</v>
@@ -2180,39 +2427,39 @@
         <v>44</v>
       </c>
       <c r="K27" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="L27" s="3">
+        <v>4.0600000000000002E-3</v>
+      </c>
+      <c r="M27" s="3">
+        <v>4.0600000000000002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="L27" s="1">
-        <v>4.0600000000000002E-3</v>
-      </c>
-      <c r="M27" s="1">
-        <v>4.0600000000000002E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F28" s="1">
+      <c r="F28" s="3">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>19</v>
@@ -2221,39 +2468,39 @@
         <v>58</v>
       </c>
       <c r="K28" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.13983999999999999</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.13983999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="L28" s="1">
-        <v>0.13983999999999999</v>
-      </c>
-      <c r="M28" s="1">
-        <v>0.13983999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>19</v>
@@ -2262,39 +2509,39 @@
         <v>44</v>
       </c>
       <c r="K29" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="L29" s="3">
+        <v>1.4E-3</v>
+      </c>
+      <c r="M29" s="3">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="L29" s="1">
-        <v>1.4E-3</v>
-      </c>
-      <c r="M29" s="1">
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F30" s="1">
+      <c r="F30" s="3">
         <v>2</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>19</v>
@@ -2303,72 +2550,80 @@
         <v>36</v>
       </c>
       <c r="K30" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="L30" s="3">
+        <v>2.2370000000000001E-2</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0.22375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="L30" s="1">
-        <v>2.2370000000000001E-2</v>
-      </c>
-      <c r="M30" s="1">
-        <v>0.22375</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F31" s="1">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="I31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F32" s="1">
-        <v>2</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="H32" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>19</v>
@@ -2377,184 +2632,240 @@
         <v>36</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="L32" s="1">
+        <v>196</v>
+      </c>
+      <c r="L32" s="3">
         <v>0.65725999999999996</v>
       </c>
-      <c r="M32" s="1">
+      <c r="M32" s="3">
         <v>1.31</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F33" s="1">
+      <c r="F33" s="3">
         <v>1</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="G33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L33" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F34" s="1">
+      <c r="F34" s="3">
         <v>1</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="G34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="L34" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F35" s="1">
+      <c r="F35" s="3">
         <v>1</v>
       </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
+      <c r="G35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L35" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M35" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="2" t="s">
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F36" s="1">
-        <v>1</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="K36" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="L36" s="1">
+        <v>213</v>
+      </c>
+      <c r="L36" s="3">
         <v>6.9899999999999997E-3</v>
       </c>
-      <c r="M36" s="1">
+      <c r="M36" s="3">
         <v>6.9899999999999997E-3</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3">
         <v>1</v>
       </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
+      <c r="G37" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="L37" s="3">
+        <v>5.28</v>
+      </c>
+      <c r="M37" s="3">
+        <v>5.28</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="H38" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>19</v>
@@ -2563,89 +2874,117 @@
         <v>44</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="L38" s="1">
+        <v>222</v>
+      </c>
+      <c r="L38" s="3">
         <v>0.10642</v>
       </c>
-      <c r="M38" s="1">
+      <c r="M38" s="3">
         <v>0.10642</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1">
+      <c r="E39" s="3"/>
+      <c r="F39" s="3">
         <v>1</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
+      <c r="G39" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="L39" s="3">
+        <v>3.27</v>
+      </c>
+      <c r="M39" s="3">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1">
+      <c r="E40" s="3"/>
+      <c r="F40" s="3">
         <v>2</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
+      <c r="G40" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="L40" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M40" s="3">
+        <v>1.1200000000000001</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F41" s="1">
+      <c r="F41" s="3">
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>19</v>
@@ -2654,64 +2993,78 @@
         <v>36</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="L41" s="1">
+        <v>240</v>
+      </c>
+      <c r="L41" s="3">
         <v>1.0900000000000001</v>
       </c>
-      <c r="M41" s="1">
+      <c r="M41" s="3">
         <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1">
+      <c r="E42" s="3"/>
+      <c r="F42" s="3">
         <v>8</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
+      <c r="G42" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="L42" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="M42" s="3">
+        <v>6.72</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="F43" s="1">
+      <c r="F43" s="3">
         <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>19</v>
@@ -2720,47 +3073,55 @@
         <v>58</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="L43" s="1">
+        <v>250</v>
+      </c>
+      <c r="L43" s="3">
         <v>3.97</v>
       </c>
-      <c r="M43" s="1">
+      <c r="M43" s="3">
         <v>3.97</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F44" s="1">
-        <v>1</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="H44" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0.92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>